<commit_message>
changed solution exported to add capacity report. Also, changed changed maint example in template_in.
</commit_message>
<xml_diff>
--- a/data/template/201902141830_2/template_in.xlsx
+++ b/data/template/201902141830_2/template_in.xlsx
@@ -4336,7 +4336,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4532,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="237.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
some corrections to heuristics, cleaning of template, correction on gantt generation, version bump.
</commit_message>
<xml_diff>
--- a/data/template/201902141830_2/template_in.xlsx
+++ b/data/template/201902141830_2/template_in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="maintenances" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="149">
   <si>
     <t xml:space="preserve">maint</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">BH_tol</t>
   </si>
   <si>
-    <t xml:space="preserve">capacite</t>
-  </si>
-  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -401,37 +398,10 @@
     <t xml:space="preserve">Valeur</t>
   </si>
   <si>
-    <t xml:space="preserve">maint_weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unavail_weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_elapsed_time</t>
-  </si>
-  <si>
     <t xml:space="preserve">min_usage_period</t>
   </si>
   <si>
-    <t xml:space="preserve">min_avail_value</t>
-  </si>
-  <si>
     <t xml:space="preserve">default_type2_capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nb_planes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deliveries_per_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lots_per_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_age_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_hours_year</t>
   </si>
   <si>
     <t xml:space="preserve">num_period</t>
@@ -509,7 +479,7 @@
 Il y a 7 mois entre le deux visites VG. Comme nous avons une tolérance de 2 mois, c’est aussi une distance acceptable. On aurait aussi pu faire la deuxième visite VG un mois plus tard, le 2019-07 pour avoir une distance entre les deux de 8 mois.
 Les valeurs pour M sont : BC=60; BC_tol=5.
 Entre la dernière visite M faite avant le début de l'horizon et la visite affectée, il y a 60 mois piles : le compteur à 1 sur la colonne 'M_p' le confirme. C'est une distance acceptable. On pourrait aussi déplacer la visite M quelques (4) mois en avant et garder une solution acceptable.
-Pourtant, il y a seulement 2 mois entre la deuxième visite VG et la visite M, ce n'est pas un distance acceptable.
+Pourtant, il y a seulement 2 mois entre la deuxième visite VG et la visite M, ce n'est pas une distance acceptable.
 Une possible solution pour ce planning peut être de déplacer la visite M 2 mois plus tôt. Comme cela on aura seulement une visite VG et une visite M qui seront cohérentes entre elles et avec les visites précédentes.
 </t>
   </si>
@@ -631,18 +601,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,13 +644,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>4</v>
@@ -693,22 +661,19 @@
       <c r="E2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="0" t="n">
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -719,25 +684,22 @@
       <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -748,25 +710,22 @@
       <c r="D4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="I4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -777,19 +736,16 @@
       <c r="F5" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="0" t="n">
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="0" t="n">
+      <c r="I5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -822,27 +778,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>-693</v>
@@ -850,32 +806,32 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>-483</v>
@@ -883,13 +839,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>-193</v>
@@ -897,32 +853,32 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>-375</v>
@@ -930,13 +886,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>-531</v>
@@ -944,32 +900,32 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>-111</v>
@@ -977,13 +933,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>-928</v>
@@ -991,32 +947,32 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>-213</v>
@@ -1024,13 +980,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>-579</v>
@@ -1038,32 +994,32 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>-91</v>
@@ -1071,13 +1027,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>-432</v>
@@ -1085,32 +1041,32 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>-136</v>
@@ -1118,13 +1074,13 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>-475</v>
@@ -1132,32 +1088,32 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>-283</v>
@@ -1165,13 +1121,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>-800</v>
@@ -1179,32 +1135,32 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>-464</v>
@@ -1212,13 +1168,13 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>-601</v>
@@ -1226,32 +1182,32 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>-304</v>
@@ -1259,13 +1215,13 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>48</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>-981</v>
@@ -1273,32 +1229,32 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>-237</v>
@@ -1306,13 +1262,13 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>-506</v>
@@ -1320,32 +1276,32 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>-201</v>
@@ -1353,13 +1309,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>-104</v>
@@ -1367,32 +1323,32 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>-261</v>
@@ -1400,13 +1356,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>-817</v>
@@ -1414,32 +1370,32 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>-368</v>
@@ -1447,13 +1403,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>-180</v>
@@ -1461,32 +1417,32 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>-23</v>
@@ -1494,13 +1450,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>-246</v>
@@ -1508,32 +1464,32 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>-162</v>
@@ -1541,13 +1497,13 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>-729</v>
@@ -1555,32 +1511,32 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>-339</v>
@@ -1588,13 +1544,13 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>-435</v>
@@ -1602,32 +1558,32 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>-263</v>
@@ -1635,13 +1591,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>-188</v>
@@ -1649,32 +1605,32 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>-409</v>
@@ -1682,13 +1638,13 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>-338</v>
@@ -1696,32 +1652,32 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>-173</v>
@@ -1729,13 +1685,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>-298</v>
@@ -1743,32 +1699,32 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>-360</v>
@@ -1776,13 +1732,13 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>-198</v>
@@ -1790,32 +1746,32 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>-91</v>
@@ -1823,13 +1779,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>-148</v>
@@ -1837,32 +1793,32 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>-281</v>
@@ -1870,13 +1826,13 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>-563</v>
@@ -1884,32 +1840,32 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>-445</v>
@@ -1917,13 +1873,13 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>-371</v>
@@ -1931,32 +1887,32 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>-304</v>
@@ -1964,13 +1920,13 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>-294</v>
@@ -1978,32 +1934,32 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>-216</v>
@@ -2011,13 +1967,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B102" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>-367</v>
@@ -2025,32 +1981,32 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>-278</v>
@@ -2058,13 +2014,13 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>-42</v>
@@ -2072,32 +2028,32 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>-401</v>
@@ -2105,13 +2061,13 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>-154</v>
@@ -2119,32 +2075,32 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D113" s="0" t="n">
         <v>-249</v>
@@ -2152,13 +2108,13 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D114" s="0" t="n">
         <v>-895</v>
@@ -2166,32 +2122,32 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D117" s="0" t="n">
         <v>-526</v>
@@ -2199,13 +2155,13 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="B118" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="D118" s="0" t="n">
         <v>-592</v>
@@ -2213,32 +2169,32 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D121" s="0" t="n">
         <v>-109</v>
@@ -2246,13 +2202,13 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D122" s="0" t="n">
         <v>-90</v>
@@ -2260,32 +2216,32 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D125" s="0" t="n">
         <v>-174</v>
@@ -2293,13 +2249,13 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="B126" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>-1015</v>
@@ -2307,32 +2263,32 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D129" s="0" t="n">
         <v>-165</v>
@@ -2340,13 +2296,13 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>-157</v>
@@ -2354,32 +2310,32 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>-331</v>
@@ -2387,13 +2343,13 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C134" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="B134" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="D134" s="0" t="n">
         <v>-623</v>
@@ -2401,32 +2357,32 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D137" s="0" t="n">
         <v>-277</v>
@@ -2434,13 +2390,13 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>-539</v>
@@ -2448,32 +2404,32 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>-263</v>
@@ -2481,13 +2437,13 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>-770</v>
@@ -2495,32 +2451,32 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>-307</v>
@@ -2528,13 +2484,13 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B146" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C146" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="D146" s="0" t="n">
         <v>-740</v>
@@ -2542,32 +2498,32 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D149" s="0" t="n">
         <v>-375</v>
@@ -2575,13 +2531,13 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B150" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C150" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="D150" s="0" t="n">
         <v>-733</v>
@@ -2589,32 +2545,32 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>-307</v>
@@ -2622,13 +2578,13 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>-354</v>
@@ -2636,32 +2592,32 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>-431</v>
@@ -2669,13 +2625,13 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>-1139</v>
@@ -2683,32 +2639,32 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>-186</v>
@@ -2716,13 +2672,13 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B162" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C162" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="D162" s="0" t="n">
         <v>-599</v>
@@ -2730,32 +2686,32 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D165" s="0" t="n">
         <v>-274</v>
@@ -2763,13 +2719,13 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D166" s="0" t="n">
         <v>-450</v>
@@ -2777,32 +2733,32 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D169" s="0" t="n">
         <v>-169</v>
@@ -2810,13 +2766,13 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>-488</v>
@@ -2824,32 +2780,32 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D173" s="0" t="n">
         <v>-372</v>
@@ -2857,13 +2813,13 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B174" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C174" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="D174" s="0" t="n">
         <v>-984</v>
@@ -2871,32 +2827,32 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D177" s="0" t="n">
         <v>-375</v>
@@ -2904,13 +2860,13 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D178" s="0" t="n">
         <v>-923</v>
@@ -2918,32 +2874,32 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D181" s="0" t="n">
         <v>-312</v>
@@ -2951,13 +2907,13 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="B182" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C182" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="D182" s="0" t="n">
         <v>-846</v>
@@ -2965,32 +2921,32 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>-520</v>
@@ -2998,13 +2954,13 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="B186" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C186" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="D186" s="0" t="n">
         <v>-658</v>
@@ -3012,32 +2968,32 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D189" s="0" t="n">
         <v>-260</v>
@@ -3045,13 +3001,13 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D190" s="0" t="n">
         <v>-478</v>
@@ -3059,32 +3015,32 @@
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D193" s="0" t="n">
         <v>-209</v>
@@ -3092,13 +3048,13 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B194" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C194" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="D194" s="0" t="n">
         <v>-705</v>
@@ -3106,32 +3062,32 @@
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D197" s="0" t="n">
         <v>-237</v>
@@ -3139,13 +3095,13 @@
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D198" s="0" t="n">
         <v>-383</v>
@@ -3153,32 +3109,32 @@
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D201" s="0" t="n">
         <v>-393</v>
@@ -3186,13 +3142,13 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D202" s="0" t="n">
         <v>-261</v>
@@ -3200,32 +3156,32 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D205" s="0" t="n">
         <v>-245</v>
@@ -3233,13 +3189,13 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D206" s="0" t="n">
         <v>-474</v>
@@ -3247,32 +3203,32 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D209" s="0" t="n">
         <v>-208</v>
@@ -3280,13 +3236,13 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D210" s="0" t="n">
         <v>-847</v>
@@ -3294,32 +3250,32 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D213" s="0" t="n">
         <v>-176</v>
@@ -3327,13 +3283,13 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D214" s="0" t="n">
         <v>-742</v>
@@ -3341,32 +3297,32 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D217" s="0" t="n">
         <v>-231</v>
@@ -3374,13 +3330,13 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D218" s="0" t="n">
         <v>-201</v>
@@ -3388,32 +3344,32 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D221" s="0" t="n">
         <v>-130</v>
@@ -3421,13 +3377,13 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D222" s="0" t="n">
         <v>-403</v>
@@ -3435,32 +3391,32 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D225" s="0" t="n">
         <v>-354</v>
@@ -3468,13 +3424,13 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D226" s="0" t="n">
         <v>-894</v>
@@ -3482,32 +3438,32 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D229" s="0" t="n">
         <v>-216</v>
@@ -3515,13 +3471,13 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C230" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="B230" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C230" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="D230" s="0" t="n">
         <v>-159</v>
@@ -3529,32 +3485,32 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D233" s="0" t="n">
         <v>-195</v>
@@ -3562,13 +3518,13 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="B234" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C234" s="0" t="s">
-        <v>121</v>
       </c>
       <c r="D234" s="0" t="n">
         <v>-168</v>
@@ -3576,32 +3532,32 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D237" s="0" t="n">
         <v>-205</v>
@@ -3609,13 +3565,13 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D238" s="0" t="n">
         <v>-739</v>
@@ -3623,32 +3579,32 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D241" s="0" t="n">
         <v>-125</v>
@@ -3670,10 +3626,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3684,42 +3640,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,81 +3683,18 @@
         <v>129</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="0" t="n">
         <v>4</v>
       </c>
     </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3831,15 +3724,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -3847,7 +3740,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -3855,7 +3748,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -3863,7 +3756,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -3871,7 +3764,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -3879,7 +3772,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -3887,7 +3780,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -3895,7 +3788,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -3903,7 +3796,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -3911,7 +3804,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -3919,7 +3812,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -3927,7 +3820,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -3935,7 +3828,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -3943,7 +3836,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -3951,7 +3844,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -3959,7 +3852,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -3967,7 +3860,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -3975,7 +3868,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -3983,7 +3876,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -3991,7 +3884,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -3999,7 +3892,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -4007,7 +3900,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -4015,7 +3908,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -4023,7 +3916,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -4031,7 +3924,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -4039,7 +3932,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -4047,7 +3940,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -4055,7 +3948,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -4063,7 +3956,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -4071,7 +3964,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -4079,7 +3972,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -4087,7 +3980,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -4095,7 +3988,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -4103,7 +3996,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -4111,7 +4004,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -4119,7 +4012,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -4127,7 +4020,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -4135,7 +4028,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -4143,7 +4036,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -4151,7 +4044,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -4159,7 +4052,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -4167,7 +4060,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -4175,7 +4068,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -4183,7 +4076,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -4191,7 +4084,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -4199,7 +4092,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -4207,7 +4100,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -4215,7 +4108,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -4223,7 +4116,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -4231,7 +4124,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -4239,7 +4132,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -4247,7 +4140,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -4255,7 +4148,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -4263,7 +4156,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -4271,7 +4164,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -4279,7 +4172,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -4287,7 +4180,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -4295,7 +4188,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -4303,7 +4196,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -4311,7 +4204,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -4335,8 +4228,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4351,27 +4244,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>846</v>
@@ -4385,7 +4278,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>831</v>
@@ -4402,7 +4295,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>816</v>
@@ -4416,7 +4309,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>801</v>
@@ -4430,7 +4323,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>786</v>
@@ -4444,7 +4337,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>771</v>
@@ -4458,7 +4351,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>756</v>
@@ -4472,7 +4365,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>741</v>
@@ -4486,7 +4379,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>726</v>
@@ -4503,7 +4396,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>711</v>
@@ -4517,7 +4410,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1000</v>
@@ -4534,7 +4427,7 @@
     </row>
     <row r="14" customFormat="false" ht="288.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4549,27 +4442,27 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>846</v>
@@ -4583,7 +4476,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>831</v>
@@ -4600,7 +4493,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>816</v>
@@ -4614,7 +4507,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>801</v>
@@ -4628,7 +4521,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>786</v>
@@ -4642,7 +4535,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>771</v>
@@ -4656,7 +4549,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>756</v>
@@ -4670,7 +4563,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>741</v>
@@ -4684,7 +4577,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1000</v>
@@ -4701,7 +4594,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B25+$B$24-$B$23</f>
@@ -4716,7 +4609,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">B26+$B$24-$B$23</f>

</xml_diff>